<commit_message>
Add import excel tests
</commit_message>
<xml_diff>
--- a/src/test/resources/files/listadoTest.xlsx
+++ b/src/test/resources/files/listadoTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joan.juan.belda\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E134893-B6BF-4ABE-A698-5F3E60DDEDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1BAF2B-FB2F-40AC-B439-854924B58BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3150" yWindow="2520" windowWidth="19425" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,79 +25,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Taula 2</t>
   </si>
   <si>
-    <t>Mesa 4</t>
-  </si>
-  <si>
-    <t>Mesa 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesa 7  </t>
-  </si>
-  <si>
     <t>Antonio</t>
   </si>
   <si>
-    <t>Pepe</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Alfredo</t>
-  </si>
-  <si>
-    <t>Amaia</t>
-  </si>
-  <si>
-    <t>Pepa</t>
-  </si>
-  <si>
     <t>Pepe-Intolerant</t>
   </si>
   <si>
     <t xml:space="preserve">Amaia-x-Celiaca </t>
   </si>
   <si>
-    <t>Pepe - x - Celiaco</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pepa - x </t>
   </si>
   <si>
-    <t>Pepa - Alegica</t>
-  </si>
-  <si>
-    <t>Jose-Celiaco-x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antonio -Celiaco- x </t>
-  </si>
-  <si>
     <t>Taula 1-Botellas</t>
   </si>
   <si>
     <t>Mesa 3 - Licores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jose </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amaia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pepe - x - Celiaco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,9 +90,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,151 +383,44 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>